<commit_message>
agregamos comentarios y el avatar
</commit_message>
<xml_diff>
--- a/Test/Test de prueba.xlsx
+++ b/Test/Test de prueba.xlsx
@@ -605,13 +605,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>